<commit_message>
catching more jacks beta testing
</commit_message>
<xml_diff>
--- a/BulkImport/MysoftDemo(702).xlsx
+++ b/BulkImport/MysoftDemo(702).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="87">
   <si>
     <t xml:space="preserve">Starting JackID </t>
   </si>
@@ -231,6 +231,18 @@
     <t>e520050b1</t>
   </si>
   <si>
+    <t>H991122AA</t>
+  </si>
+  <si>
+    <t>H991122AA-d</t>
+  </si>
+  <si>
+    <t>A041363AA-D</t>
+  </si>
+  <si>
+    <t>A041363AA</t>
+  </si>
+  <si>
     <t>WIRELESS-AP-INDOOR</t>
   </si>
   <si>
@@ -267,19 +279,25 @@
     <t>A120353B1-DW, PG103005</t>
   </si>
   <si>
-    <t>A041363AA-VD, Manual update needed, two results (no ap)</t>
+    <t>A01019CUPSB1-D, Manual update needed, two results (no ap)</t>
+  </si>
+  <si>
+    <t>A01019CUPSB1-D, 0007</t>
+  </si>
+  <si>
+    <t>A442448UPSB1-D, 0007</t>
   </si>
   <si>
     <t>Manual Update needed</t>
   </si>
   <si>
-    <t>A01019CUPSB1-D, Manual update needed, two results (no ap)</t>
-  </si>
-  <si>
-    <t>A01019CUPSB1-D, 0007</t>
-  </si>
-  <si>
-    <t>A442448UPSB1-D, 0007</t>
+    <t>H991122AA-DW, PG112220</t>
+  </si>
+  <si>
+    <t>A041363AA-D, PG103139</t>
+  </si>
+  <si>
+    <t>A041363AA, Manual update needed, two results (no ap)</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9EBD13-F7C7-43A4-A92A-4BF2D4A07456}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1233,10 +1251,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1257,7 +1275,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1265,26 +1283,26 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1361,18 +1379,18 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1380,8 +1398,58 @@
         <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1390,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B1A0E0-C92A-42C7-B437-5220C8B399E3}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A2" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1460,7 +1528,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -1525,7 +1593,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -1537,7 +1605,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1554,7 +1622,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>36</v>
@@ -1571,7 +1639,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>36</v>
@@ -1588,7 +1656,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>36</v>
@@ -1605,7 +1673,7 @@
         <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>36</v>
@@ -1622,7 +1690,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>36</v>
@@ -1639,7 +1707,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>36</v>
@@ -1656,7 +1724,7 @@
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>36</v>
@@ -1673,7 +1741,7 @@
         <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>36</v>
@@ -1690,7 +1758,7 @@
         <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>36</v>
@@ -1704,16 +1772,16 @@
         <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1721,13 +1789,13 @@
         <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>8</v>
@@ -1738,6 +1806,26 @@
         <v>63</v>
       </c>
       <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>